<commit_message>
Fixed notebook and dictionary
</commit_message>
<xml_diff>
--- a/ACS Feature Dictionary.xlsx
+++ b/ACS Feature Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41d509ce3db0a387/GitHub/homelessness_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{33FDBB2A-7EAF-DF49-B74D-D759D9DF24FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A6E3262-C76F-564D-BC40-B5CBDC53ED97}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{33FDBB2A-7EAF-DF49-B74D-D759D9DF24FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E5797C-80B8-4946-9AF6-BEA8861D7AC0}"/>
   <bookViews>
-    <workbookView xWindow="19060" yWindow="4060" windowWidth="28040" windowHeight="17440" xr2:uid="{0EFEA481-7FE1-E54E-A2F9-5275F1F78CBD}"/>
+    <workbookView xWindow="29640" yWindow="4060" windowWidth="17460" windowHeight="17440" xr2:uid="{0EFEA481-7FE1-E54E-A2F9-5275F1F78CBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>B01001_003E</t>
-  </si>
-  <si>
     <t>Alias</t>
   </si>
   <si>
@@ -618,6 +615,9 @@
   </si>
   <si>
     <t>Univeristy of Oklahoma</t>
+  </si>
+  <si>
+    <t>B01001_026E</t>
   </si>
 </sst>
 </file>
@@ -690,6 +690,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5584658C-F9DB-DC49-84D7-0324BE43DD4F}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1012,12 +1016,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1033,16 +1037,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1053,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -1063,7 +1067,7 @@
         <v>pop_tot_pcp</v>
       </c>
       <c r="F8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1074,7 +1078,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -1084,7 +1088,7 @@
         <v>pop_male_pcp</v>
       </c>
       <c r="F9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1095,17 +1099,17 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>193</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>pop_female_pcp</v>
       </c>
       <c r="F10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1113,20 +1117,20 @@
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>35</v>
-      </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
         <v>pop_white_pcp</v>
       </c>
       <c r="F11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1134,20 +1138,20 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
         <v>pop_black_pcp</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1155,20 +1159,20 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>20</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
         <v>pop_aiak_pcp</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1176,20 +1180,20 @@
         <v>4</v>
       </c>
       <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" t="s">
-        <v>24</v>
-      </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
         <v>pop_asian_pcp</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1197,20 +1201,20 @@
         <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
         <v>pop_hipi_pcp</v>
       </c>
       <c r="F15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1218,20 +1222,20 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" t="s">
         <v>28</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>29</v>
       </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
         <v>pop_other_pcp</v>
       </c>
       <c r="F16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1239,20 +1243,20 @@
         <v>4</v>
       </c>
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" t="s">
-        <v>33</v>
-      </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
         <v>pop_mult_pcp</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1260,20 +1264,20 @@
         <v>4</v>
       </c>
       <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
         <v>pop_hisp_pcp</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1281,349 +1285,349 @@
         <v>4</v>
       </c>
       <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
-        <v>41</v>
-      </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
         <v>pop_medage_pcp</v>
       </c>
       <c r="F19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
         <v>44</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>45</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="str">
+        <f t="shared" si="0"/>
+        <v>mob_tot_pcp</v>
+      </c>
+      <c r="F20" t="s">
         <v>46</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>mob_tot_pcp</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" t="s">
         <v>48</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>49</v>
       </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
         <v>mob_nomove_pcp</v>
       </c>
       <c r="F21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
         <v>51</v>
       </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>52</v>
-      </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v>mob_samecounty_pcp</v>
       </c>
       <c r="F22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
-        <v>54</v>
-      </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v>mob_diffcounty_pcp</v>
       </c>
       <c r="F23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
         <v>56</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>57</v>
       </c>
-      <c r="D24" t="s">
-        <v>58</v>
-      </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>mob_diffstate_pcp</v>
       </c>
       <c r="F24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" t="s">
         <v>60</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>61</v>
       </c>
-      <c r="D25" t="s">
-        <v>62</v>
-      </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
         <v>mob_diffcntry_pcp</v>
       </c>
       <c r="F25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
         <v>66</v>
       </c>
-      <c r="D26" t="s">
-        <v>67</v>
-      </c>
       <c r="E26" t="str">
         <f t="shared" si="0"/>
         <v>pov_total_pcp</v>
       </c>
       <c r="F26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
         <v>68</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="D27" t="s">
-        <v>70</v>
-      </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
         <v>pov_u50_pcp</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
         <v>pov_50t74_pcp</v>
       </c>
       <c r="F28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
         <v>pov_75t99_pcp</v>
       </c>
       <c r="F29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
         <v>pov_100t124_pcp</v>
       </c>
       <c r="F30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>pov_125t149_pcp</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
         <v>pov_150t174_pcp</v>
       </c>
       <c r="F32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
         <v>pov_175t184_pcp</v>
       </c>
       <c r="F33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
+        <v>90</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="0"/>
+        <v>pov_185t199_pcp</v>
+      </c>
+      <c r="F34" t="s">
         <v>91</v>
-      </c>
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" t="str">
-        <f t="shared" si="0"/>
-        <v>pov_185t199_pcp</v>
-      </c>
-      <c r="F34" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" t="s">
         <v>93</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>94</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>95</v>
-      </c>
-      <c r="D35" t="s">
-        <v>96</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -1632,247 +1636,247 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" t="s">
         <v>97</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>98</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>99</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="str">
+        <f t="shared" si="0"/>
+        <v>asst_total_pcp</v>
+      </c>
+      <c r="F36" t="s">
         <v>100</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>asst_total_pcp</v>
-      </c>
-      <c r="F36" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B37" t="s">
+        <v>101</v>
+      </c>
+      <c r="C37" t="s">
         <v>102</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
-        <v>104</v>
-      </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
         <v>asst_rcvd_pcp</v>
       </c>
       <c r="F37" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
         <v>105</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>106</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>107</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="str">
+        <f t="shared" si="0"/>
+        <v>empl_tot_pcp</v>
+      </c>
+      <c r="F38" t="s">
         <v>108</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>empl_tot_pcp</v>
-      </c>
-      <c r="F38" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
         <v>110</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>111</v>
       </c>
-      <c r="D39" t="s">
-        <v>112</v>
-      </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
         <v>empl_notinlabor_pcp</v>
       </c>
       <c r="F39" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B40" t="s">
         <v>113</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>114</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>115</v>
       </c>
-      <c r="D40" t="s">
-        <v>116</v>
-      </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
         <v>occu_tot_pcp</v>
       </c>
       <c r="F40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
+        <v>119</v>
+      </c>
+      <c r="C41" t="s">
         <v>120</v>
       </c>
-      <c r="C41" t="s">
-        <v>121</v>
-      </c>
       <c r="D41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
         <v>occu_vacant_pcp</v>
       </c>
       <c r="F41" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" t="s">
         <v>122</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>124</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="str">
+        <f t="shared" si="0"/>
+        <v>tenure_tot_pcp</v>
+      </c>
+      <c r="F42" t="s">
         <v>125</v>
-      </c>
-      <c r="E42" t="str">
-        <f t="shared" si="0"/>
-        <v>tenure_tot_pcp</v>
-      </c>
-      <c r="F42" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" t="s">
         <v>127</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>128</v>
       </c>
-      <c r="D43" t="s">
-        <v>129</v>
-      </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
         <v>tenure_rent_pcp</v>
       </c>
       <c r="F43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>129</v>
+      </c>
+      <c r="B44" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" t="s">
         <v>130</v>
       </c>
-      <c r="B44" t="s">
-        <v>114</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>131</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="str">
+        <f t="shared" si="0"/>
+        <v>vcncy_tot_pcp</v>
+      </c>
+      <c r="F44" t="s">
         <v>132</v>
-      </c>
-      <c r="E44" t="str">
-        <f t="shared" si="0"/>
-        <v>vcncy_tot_pcp</v>
-      </c>
-      <c r="F44" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" t="s">
         <v>134</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>135</v>
       </c>
-      <c r="D45" t="s">
-        <v>136</v>
-      </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
         <v>vcncy_forrent_pcp</v>
       </c>
       <c r="F45" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
+        <v>136</v>
+      </c>
+      <c r="C46" t="s">
         <v>137</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>138</v>
       </c>
-      <c r="D46" t="s">
-        <v>139</v>
-      </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
         <v>vcncy_forsale_pcp</v>
       </c>
       <c r="F46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" t="s">
         <v>140</v>
-      </c>
-      <c r="D47" t="s">
-        <v>141</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -1881,16 +1885,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B48" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" t="s">
         <v>142</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>143</v>
-      </c>
-      <c r="D48" t="s">
-        <v>144</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -1899,16 +1903,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49" t="s">
         <v>145</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>146</v>
-      </c>
-      <c r="D49" t="s">
-        <v>147</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -1917,16 +1921,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
+        <v>148</v>
+      </c>
+      <c r="B50" t="s">
         <v>149</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
+        <v>155</v>
+      </c>
+      <c r="D50" t="s">
         <v>150</v>
-      </c>
-      <c r="C50" t="s">
-        <v>156</v>
-      </c>
-      <c r="D50" t="s">
-        <v>151</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -1935,16 +1939,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C51" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" t="s">
         <v>152</v>
-      </c>
-      <c r="D51" t="s">
-        <v>153</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -1953,16 +1957,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C52" t="s">
+        <v>153</v>
+      </c>
+      <c r="D52" t="s">
         <v>154</v>
-      </c>
-      <c r="D52" t="s">
-        <v>155</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
@@ -1971,233 +1975,233 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
+        <v>156</v>
+      </c>
+      <c r="B53" t="s">
         <v>157</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>158</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>159</v>
       </c>
-      <c r="D53" t="s">
-        <v>160</v>
-      </c>
       <c r="E53" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_tot_pcp</v>
       </c>
       <c r="F53" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B54" t="s">
+        <v>160</v>
+      </c>
+      <c r="C54" t="s">
         <v>161</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>162</v>
       </c>
-      <c r="D54" t="s">
-        <v>163</v>
-      </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_u10_pcp</v>
       </c>
       <c r="F54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" t="s">
         <v>164</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>165</v>
       </c>
-      <c r="D55" t="s">
-        <v>166</v>
-      </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_10t14_pcp</v>
       </c>
       <c r="F55" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B56" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56" t="s">
         <v>167</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>168</v>
       </c>
-      <c r="D56" t="s">
-        <v>169</v>
-      </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_15t19_pcp</v>
       </c>
       <c r="F56" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B57" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" t="s">
         <v>170</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>171</v>
       </c>
-      <c r="D57" t="s">
-        <v>172</v>
-      </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_20t24_pcp</v>
       </c>
       <c r="F57" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B58" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C58" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" t="s">
         <v>173</v>
       </c>
-      <c r="D58" t="s">
-        <v>174</v>
-      </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_25t29_pcp</v>
       </c>
       <c r="F58" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B59" t="s">
+        <v>175</v>
+      </c>
+      <c r="C59" t="s">
         <v>176</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>177</v>
       </c>
-      <c r="D59" t="s">
-        <v>178</v>
-      </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_30t34_pcp</v>
       </c>
       <c r="F59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" t="s">
         <v>179</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>180</v>
       </c>
-      <c r="D60" t="s">
-        <v>181</v>
-      </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_35t39_pcp</v>
       </c>
       <c r="F60" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B61" t="s">
+        <v>181</v>
+      </c>
+      <c r="C61" t="s">
         <v>182</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>183</v>
       </c>
-      <c r="D61" t="s">
-        <v>184</v>
-      </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_40t49_pcp</v>
       </c>
       <c r="F61" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B62" t="s">
+        <v>184</v>
+      </c>
+      <c r="C62" t="s">
         <v>185</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>186</v>
       </c>
-      <c r="D62" t="s">
-        <v>187</v>
-      </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_50plus_pcp</v>
       </c>
       <c r="F62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
+        <v>187</v>
+      </c>
+      <c r="C63" t="s">
         <v>188</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>189</v>
       </c>
-      <c r="D63" t="s">
+      <c r="E63" t="str">
+        <f t="shared" si="0"/>
+        <v>rentpct_median_pcp</v>
+      </c>
+      <c r="F63" t="s">
         <v>190</v>
-      </c>
-      <c r="E63" t="str">
-        <f t="shared" si="0"/>
-        <v>rentpct_median_pcp</v>
-      </c>
-      <c r="F63" t="s">
-        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final version of ACS data grabber
</commit_message>
<xml_diff>
--- a/ACS Feature Dictionary.xlsx
+++ b/ACS Feature Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/41d509ce3db0a387/GitHub/homelessness_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{33FDBB2A-7EAF-DF49-B74D-D759D9DF24FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5E5797C-80B8-4946-9AF6-BEA8861D7AC0}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{A2FCDE5B-3973-8141-A716-3EEA1A265AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{266F4611-B4DF-B041-BCD7-4CB5AB101E3A}"/>
   <bookViews>
-    <workbookView xWindow="29640" yWindow="4060" windowWidth="17460" windowHeight="17440" xr2:uid="{0EFEA481-7FE1-E54E-A2F9-5275F1F78CBD}"/>
+    <workbookView xWindow="10840" yWindow="2880" windowWidth="27380" windowHeight="17440" xr2:uid="{0EFEA481-7FE1-E54E-A2F9-5275F1F78CBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={21BDD9E4-211D-4A46-B980-77AD8787EECA}</author>
+  </authors>
+  <commentList>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{21BDD9E4-211D-4A46-B980-77AD8787EECA}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Inclusion of “remove” in the value means it is not to be included in final features</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="184">
   <si>
     <t>ACS Data Dictionary</t>
   </si>
@@ -164,9 +182,6 @@
     <t>Mobility</t>
   </si>
   <si>
-    <t>Divide by B01001_001E</t>
-  </si>
-  <si>
     <t>Total population</t>
   </si>
   <si>
@@ -176,9 +191,6 @@
     <t>B07001_001E</t>
   </si>
   <si>
-    <t>Divide by B07001_001E</t>
-  </si>
-  <si>
     <t>Non-movers</t>
   </si>
   <si>
@@ -227,15 +239,9 @@
     <t>Per Capita Value</t>
   </si>
   <si>
-    <t>Per Capita Calculation</t>
-  </si>
-  <si>
     <t>Poverty Level</t>
   </si>
   <si>
-    <t>pov_total</t>
-  </si>
-  <si>
     <t>B17002_001E</t>
   </si>
   <si>
@@ -311,9 +317,6 @@
     <t>pov_185t199</t>
   </si>
   <si>
-    <t>Divide by B17002_002E</t>
-  </si>
-  <si>
     <t>Median Earnings</t>
   </si>
   <si>
@@ -332,15 +335,9 @@
     <t>Total households</t>
   </si>
   <si>
-    <t>asst_total</t>
-  </si>
-  <si>
     <t>B22001_001E</t>
   </si>
   <si>
-    <t>Divide by B22001_001E</t>
-  </si>
-  <si>
     <t>Received assistance</t>
   </si>
   <si>
@@ -362,18 +359,12 @@
     <t>B23025_001E</t>
   </si>
   <si>
-    <t>Divide by B23025_001E</t>
-  </si>
-  <si>
     <t>Not in labor force</t>
   </si>
   <si>
     <t>empl_notinlabor</t>
   </si>
   <si>
-    <t>B23025_003E</t>
-  </si>
-  <si>
     <t>Housing-Occupancy</t>
   </si>
   <si>
@@ -386,15 +377,9 @@
     <t>B25002_001E</t>
   </si>
   <si>
-    <t>Divide by B25002_002E</t>
-  </si>
-  <si>
     <t>B25002_003E</t>
   </si>
   <si>
-    <t>Divide by B25001_002E</t>
-  </si>
-  <si>
     <t>Vacant</t>
   </si>
   <si>
@@ -413,9 +398,6 @@
     <t>B25003_001E</t>
   </si>
   <si>
-    <t>Divide by B25003_001E</t>
-  </si>
-  <si>
     <t>Rented units</t>
   </si>
   <si>
@@ -434,9 +416,6 @@
     <t>B25004_001E</t>
   </si>
   <si>
-    <t>Divide by B25004_001E</t>
-  </si>
-  <si>
     <t>For rent</t>
   </si>
   <si>
@@ -608,9 +587,6 @@
     <t>B25071_001E</t>
   </si>
   <si>
-    <t>Divide by B25070_001E</t>
-  </si>
-  <si>
     <t>Matthew Beattie</t>
   </si>
   <si>
@@ -618,6 +594,18 @@
   </si>
   <si>
     <t>B01001_026E</t>
+  </si>
+  <si>
+    <t>pov_tot</t>
+  </si>
+  <si>
+    <t>asst_tot</t>
+  </si>
+  <si>
+    <t>B23025_007E</t>
+  </si>
+  <si>
+    <t>Per Capita Divisor</t>
   </si>
 </sst>
 </file>
@@ -648,12 +636,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -668,13 +662,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -693,7 +688,9 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Matthew Beattie" id="{9B360344-BABE-D941-AB92-C64814ABE6EE}" userId="41d509ce3db0a387" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,22 +988,30 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E7" dT="2023-06-19T18:30:50.95" personId="{9B360344-BABE-D941-AB92-C64814ABE6EE}" id="{21BDD9E4-211D-4A46-B980-77AD8787EECA}">
+    <text>Inclusion of “remove” in the value means it is not to be included in final features</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5584658C-F9DB-DC49-84D7-0324BE43DD4F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5584658C-F9DB-DC49-84D7-0324BE43DD4F}">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="16.1640625" customWidth="1"/>
     <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
@@ -1016,12 +1021,12 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1043,10 +1048,10 @@
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1062,12 +1067,12 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="str">
-        <f>_xlfn.CONCAT(C8,"_pcp")</f>
-        <v>pop_tot_pcp</v>
+      <c r="E8" s="4" t="str">
+        <f>_xlfn.CONCAT(C8,"_pcp_remove")</f>
+        <v>pop_tot_pcp_remove</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1088,7 +1093,7 @@
         <v>pop_male_pcp</v>
       </c>
       <c r="F9" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1102,14 +1107,14 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
         <v>pop_female_pcp</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1130,7 +1135,7 @@
         <v>pop_white_pcp</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1151,7 +1156,7 @@
         <v>pop_black_pcp</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1172,7 +1177,7 @@
         <v>pop_aiak_pcp</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1193,7 +1198,7 @@
         <v>pop_asian_pcp</v>
       </c>
       <c r="F14" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1214,7 +1219,7 @@
         <v>pop_hipi_pcp</v>
       </c>
       <c r="F15" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1235,7 +1240,7 @@
         <v>pop_other_pcp</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -1256,7 +1261,7 @@
         <v>pop_mult_pcp</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1277,7 +1282,7 @@
         <v>pop_hisp_pcp</v>
       </c>
       <c r="F18" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1297,29 +1302,26 @@
         <f t="shared" si="0"/>
         <v>pop_medage_pcp</v>
       </c>
-      <c r="F19" t="s">
-        <v>42</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>41</v>
       </c>
       <c r="B20" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
         <v>43</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>44</v>
       </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>mob_tot_pcp</v>
+      <c r="E20" s="4" t="str">
+        <f>_xlfn.CONCAT(C20,"_pcp_remove")</f>
+        <v>mob_tot_pcp_remove</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1327,20 +1329,20 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
         <v>47</v>
       </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" t="s">
-        <v>49</v>
-      </c>
       <c r="E21" t="str">
         <f t="shared" si="0"/>
         <v>mob_nomove_pcp</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1348,20 +1350,20 @@
         <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="0"/>
         <v>mob_samecounty_pcp</v>
       </c>
       <c r="F22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1369,20 +1371,20 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="0"/>
         <v>mob_diffcounty_pcp</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
@@ -1390,20 +1392,20 @@
         <v>41</v>
       </c>
       <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D24" t="s">
         <v>55</v>
       </c>
-      <c r="C24" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" t="s">
-        <v>57</v>
-      </c>
       <c r="E24" t="str">
         <f t="shared" si="0"/>
         <v>mob_diffstate_pcp</v>
       </c>
       <c r="F24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1411,223 +1413,223 @@
         <v>41</v>
       </c>
       <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D25" t="s">
         <v>59</v>
       </c>
-      <c r="C25" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" t="s">
-        <v>61</v>
-      </c>
       <c r="E25" t="str">
         <f t="shared" si="0"/>
         <v>mob_diffcntry_pcp</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
       <c r="C26" t="s">
-        <v>65</v>
+        <v>180</v>
       </c>
       <c r="D26" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="0"/>
-        <v>pov_total_pcp</v>
+        <v>62</v>
+      </c>
+      <c r="E26" s="4" t="str">
+        <f>_xlfn.CONCAT(C26,"_pcp_remove")</f>
+        <v>pov_tot_pcp_remove</v>
       </c>
       <c r="F26" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" t="s">
-        <v>67</v>
-      </c>
-      <c r="C27" t="s">
-        <v>68</v>
-      </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="0"/>
         <v>pov_u50_pcp</v>
       </c>
       <c r="F27" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="0"/>
         <v>pov_50t74_pcp</v>
       </c>
       <c r="F28" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D29" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="0"/>
         <v>pov_75t99_pcp</v>
       </c>
       <c r="F29" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D30" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="0"/>
         <v>pov_100t124_pcp</v>
       </c>
       <c r="F30" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D31" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="0"/>
         <v>pov_125t149_pcp</v>
       </c>
       <c r="F31" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="0"/>
         <v>pov_150t174_pcp</v>
       </c>
       <c r="F32" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D33" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="0"/>
         <v>pov_175t184_pcp</v>
       </c>
       <c r="F33" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C34" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D34" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="0"/>
         <v>pov_185t199_pcp</v>
       </c>
       <c r="F34" t="s">
-        <v>91</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C35" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D35" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="0"/>
@@ -1636,247 +1638,247 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C36" t="s">
-        <v>98</v>
+        <v>181</v>
       </c>
       <c r="D36" t="s">
-        <v>99</v>
-      </c>
-      <c r="E36" t="str">
-        <f t="shared" si="0"/>
-        <v>asst_total_pcp</v>
+        <v>93</v>
+      </c>
+      <c r="E36" s="4" t="str">
+        <f>_xlfn.CONCAT(C36,"_pcp_remove")</f>
+        <v>asst_tot_pcp_remove</v>
       </c>
       <c r="F36" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
+        <v>91</v>
+      </c>
+      <c r="B37" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
         <v>96</v>
       </c>
-      <c r="B37" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" t="s">
-        <v>103</v>
-      </c>
       <c r="E37" t="str">
         <f t="shared" si="0"/>
         <v>asst_rcvd_pcp</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B38" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
-      </c>
-      <c r="E38" t="str">
-        <f t="shared" si="0"/>
-        <v>empl_tot_pcp</v>
+        <v>100</v>
+      </c>
+      <c r="E38" s="4" t="str">
+        <f>_xlfn.CONCAT(C38,"_pcp_remove")</f>
+        <v>empl_tot_pcp_remove</v>
       </c>
       <c r="F38" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B39" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D39" t="s">
-        <v>111</v>
+        <v>182</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="0"/>
         <v>empl_notinlabor_pcp</v>
       </c>
       <c r="F39" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D40" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="0"/>
         <v>occu_tot_pcp</v>
       </c>
       <c r="F40" t="s">
-        <v>118</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D41" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="0"/>
         <v>occu_vacant_pcp</v>
       </c>
       <c r="F41" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D42" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="0"/>
         <v>tenure_tot_pcp</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="B43" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C43" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="D43" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="0"/>
         <v>tenure_rent_pcp</v>
       </c>
       <c r="F43" t="s">
-        <v>125</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="0"/>
         <v>vcncy_tot_pcp</v>
       </c>
       <c r="F44" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D45" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="0"/>
         <v>vcncy_forrent_pcp</v>
       </c>
       <c r="F45" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C46" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D46" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="0"/>
         <v>vcncy_forsale_pcp</v>
       </c>
       <c r="F46" t="s">
-        <v>132</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B47" t="s">
         <v>5</v>
       </c>
       <c r="C47" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="D47" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="0"/>
@@ -1885,16 +1887,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D48" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="0"/>
@@ -1903,16 +1905,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="0"/>
@@ -1921,16 +1923,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B50" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D50" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="0"/>
@@ -1939,16 +1941,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B51" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="C51" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="0"/>
@@ -1957,16 +1959,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="D52" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="0"/>
@@ -1975,236 +1977,234 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="C53" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="D53" t="s">
-        <v>159</v>
-      </c>
-      <c r="E53" t="str">
-        <f t="shared" si="0"/>
-        <v>rentpct_tot_pcp</v>
+        <v>146</v>
+      </c>
+      <c r="E53" s="4" t="str">
+        <f>_xlfn.CONCAT(C53,"_pcp_remove")</f>
+        <v>rentpct_tot_pcp_remove</v>
       </c>
       <c r="F53" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B54" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C54" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_u10_pcp</v>
       </c>
       <c r="F54" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B55" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="C55" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="D55" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_10t14_pcp</v>
       </c>
       <c r="F55" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="C56" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="D56" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_15t19_pcp</v>
       </c>
       <c r="F56" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
+        <v>143</v>
+      </c>
+      <c r="B57" t="s">
         <v>156</v>
       </c>
-      <c r="B57" t="s">
-        <v>169</v>
-      </c>
       <c r="C57" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="D57" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="E57" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_20t24_pcp</v>
       </c>
       <c r="F57" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B58" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="C58" t="s">
-        <v>172</v>
+        <v>159</v>
       </c>
       <c r="D58" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_25t29_pcp</v>
       </c>
       <c r="F58" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="C59" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="D59" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_30t34_pcp</v>
       </c>
       <c r="F59" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B60" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="C60" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_35t39_pcp</v>
       </c>
       <c r="F60" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B61" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C61" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="D61" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_40t49_pcp</v>
       </c>
       <c r="F61" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B62" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="C62" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="D62" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_50plus_pcp</v>
       </c>
       <c r="F62" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="B63" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="C63" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="D63" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="0"/>
         <v>rentpct_median_pcp</v>
-      </c>
-      <c r="F63" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>